<commit_message>
add change_language class and success to write data
</commit_message>
<xml_diff>
--- a/导出数据表格设计.xlsx
+++ b/导出数据表格设计.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>数据页面</t>
   </si>
@@ -43,7 +43,7 @@
     <t>brand</t>
   </si>
   <si>
-    <t>重构Title</t>
+    <t>new-title</t>
   </si>
   <si>
     <t>data-title</t>
@@ -52,43 +52,52 @@
     <t>href</t>
   </si>
   <si>
-    <t>价格</t>
-  </si>
-  <si>
-    <t>颜色1</t>
-  </si>
-  <si>
-    <t>颜色2</t>
-  </si>
-  <si>
-    <t>颜色3</t>
-  </si>
-  <si>
-    <t>颜色4</t>
-  </si>
-  <si>
-    <t>尺码</t>
-  </si>
-  <si>
-    <t>尺码表</t>
-  </si>
-  <si>
-    <t>描述</t>
-  </si>
-  <si>
-    <t>卖点</t>
-  </si>
-  <si>
-    <t>图片链接1</t>
-  </si>
-  <si>
-    <t>图片链接2</t>
-  </si>
-  <si>
-    <t>图片链接3</t>
-  </si>
-  <si>
-    <t>图片链接4</t>
+    <t>price</t>
+  </si>
+  <si>
+    <t>color1</t>
+  </si>
+  <si>
+    <t>color2</t>
+  </si>
+  <si>
+    <t>color3</t>
+  </si>
+  <si>
+    <t>color4</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>size_chert</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>bullet-point</t>
+  </si>
+  <si>
+    <t>image-url1</t>
+  </si>
+  <si>
+    <t>image-url2</t>
+  </si>
+  <si>
+    <t>image-url3</t>
+  </si>
+  <si>
+    <t>image-url4</t>
+  </si>
+  <si>
+    <t>image-url5</t>
+  </si>
+  <si>
+    <t>image-url6</t>
+  </si>
+  <si>
+    <t>image-url7</t>
   </si>
   <si>
     <t>sku-parent</t>
@@ -126,10 +135,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -166,35 +175,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -204,23 +184,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -228,14 +199,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -243,16 +221,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="8"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -264,6 +251,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -272,16 +274,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,15 +299,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -330,6 +339,150 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -342,175 +495,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,10 +550,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -565,15 +572,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -589,16 +587,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -622,17 +620,28 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,10 +653,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -656,136 +665,136 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
@@ -1171,20 +1180,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="18" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomRight" activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
   <cols>
     <col min="1" max="1" width="14.625" customWidth="1"/>
     <col min="3" max="4" width="10.125" customWidth="1"/>
+    <col min="12" max="12" width="11.5" customWidth="1"/>
+    <col min="13" max="13" width="12.625" customWidth="1"/>
+    <col min="14" max="14" width="13.75" customWidth="1"/>
+    <col min="15" max="21" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -1213,7 +1226,7 @@
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:21">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
@@ -1267,31 +1280,40 @@
       </c>
       <c r="R2" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1321,19 +1343,19 @@
   <sheetData>
     <row r="1" ht="15" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change bullet_point to dict
</commit_message>
<xml_diff>
--- a/导出数据表格设计.xlsx
+++ b/导出数据表格设计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12615"/>
+    <workbookView windowWidth="28800" windowHeight="12615" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="导出表格设计" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>数据页面</t>
   </si>
@@ -128,6 +128,21 @@
   </si>
   <si>
     <t>bullet_point5</t>
+  </si>
+  <si>
+    <t>feed_product_type</t>
+  </si>
+  <si>
+    <t>brand_name</t>
+  </si>
+  <si>
+    <t>recommended_browse_nodes</t>
+  </si>
+  <si>
+    <t>department_name</t>
+  </si>
+  <si>
+    <t>target_gender</t>
   </si>
 </sst>
 </file>
@@ -140,13 +155,19 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -312,12 +333,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD5B4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -653,10 +680,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -665,154 +692,157 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1182,12 +1212,12 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="18" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="S4" sqref="S4"/>
+      <selection pane="bottomRight" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="6"/>
@@ -1201,93 +1231,93 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
     </row>
     <row r="2" spans="1:21">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1342,19 +1372,19 @@
   </cols>
   <sheetData>
     <row r="1" ht="15" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1370,14 +1400,50 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>
+  <cols>
+    <col min="1" max="1" width="26.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" ht="15" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" ht="15" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" ht="15" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" ht="15" spans="1:1">
+      <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="5">
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="商品タイプをプルダウンから選択してください" sqref="A1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="最大50バイトまでの文字列（全角の場合16文字相当)。略さず正式ブランド・メーカー名を記入。アルファベットと(カナ)を表記" sqref="A2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="推奨値タブから適切な値を選択。" sqref="A4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="ブラウズツリーガイドに載っているコード。" sqref="A3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="次のオプションのいずれかを選択します：「男性」 「女性」 「ユニセックス」" sqref="A5"/>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>